<commit_message>
Update insurance and charity modules with multi-select component and excel upload improvements
</commit_message>
<xml_diff>
--- a/public/exele/sample.xlsx
+++ b/public/exele/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.jalilvand\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD39E4D7-B63D-4A57-A9BF-19D946BF3CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48985AA5-8162-456C-B206-201285784E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="لیست اصلی" sheetId="5" r:id="rId1"/>
@@ -23,6 +23,9 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -112,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="409">
   <si>
     <t>استان</t>
   </si>
@@ -2100,6 +2103,36 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2115,37 +2148,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2183,9 +2186,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2223,7 +2226,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2329,7 +2332,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2471,7 +2474,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2482,10 +2485,10 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="88" zoomScaleNormal="81" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
@@ -2512,85 +2515,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="25.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="81"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="91"/>
     </row>
     <row r="2" spans="1:17" ht="25.95" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="C2" s="89" t="s">
+      <c r="C2" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="D2" s="85" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="89" t="s">
+      <c r="E2" s="83" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="89" t="s">
+      <c r="F2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="89" t="s">
+      <c r="G2" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="89" t="s">
+      <c r="H2" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="I2" s="89" t="s">
+      <c r="I2" s="83" t="s">
         <v>68</v>
       </c>
-      <c r="J2" s="89" t="s">
+      <c r="J2" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="89" t="s">
+      <c r="K2" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="89" t="s">
+      <c r="L2" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="85" t="s">
+      <c r="M2" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="85"/>
-      <c r="O2" s="85"/>
-      <c r="P2" s="85"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
       <c r="Q2" s="93" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="78"/>
-      <c r="B3" s="88"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="84"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
       <c r="M3" s="48" t="s">
         <v>10</v>
       </c>
@@ -2628,15 +2631,15 @@
       <c r="P4" s="36"/>
       <c r="Q4" s="37"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="63">
         <v>2</v>
       </c>
-      <c r="B5" s="82">
+      <c r="B5" s="80">
         <v>2</v>
       </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="70"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="69"/>
       <c r="E5" s="57"/>
       <c r="F5" s="57"/>
       <c r="G5" s="2"/>
@@ -2655,9 +2658,9 @@
       <c r="A6" s="63">
         <v>3</v>
       </c>
-      <c r="B6" s="84"/>
+      <c r="B6" s="79"/>
       <c r="C6" s="59"/>
-      <c r="D6" s="71"/>
+      <c r="D6" s="69"/>
       <c r="E6" s="59"/>
       <c r="F6" s="59"/>
       <c r="G6" s="6"/>
@@ -2680,7 +2683,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="65"/>
-      <c r="D7" s="72"/>
+      <c r="D7" s="69"/>
       <c r="E7" s="65"/>
       <c r="F7" s="65"/>
       <c r="G7" s="27"/>
@@ -2699,11 +2702,11 @@
       <c r="A8" s="63">
         <v>5</v>
       </c>
-      <c r="B8" s="82">
+      <c r="B8" s="80">
         <v>4</v>
       </c>
       <c r="C8" s="57"/>
-      <c r="D8" s="70"/>
+      <c r="D8" s="69"/>
       <c r="E8" s="57"/>
       <c r="F8" s="57"/>
       <c r="G8" s="2"/>
@@ -2722,7 +2725,7 @@
       <c r="A9" s="63">
         <v>6</v>
       </c>
-      <c r="B9" s="83"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="58"/>
       <c r="D9" s="73"/>
       <c r="E9" s="58"/>
@@ -2743,7 +2746,7 @@
       <c r="A10" s="63">
         <v>7</v>
       </c>
-      <c r="B10" s="84"/>
+      <c r="B10" s="79"/>
       <c r="C10" s="59"/>
       <c r="D10" s="71"/>
       <c r="E10" s="59"/>
@@ -2786,7 +2789,7 @@
       <c r="A12" s="63">
         <v>9</v>
       </c>
-      <c r="B12" s="82">
+      <c r="B12" s="80">
         <v>6</v>
       </c>
       <c r="C12" s="57"/>
@@ -2809,7 +2812,7 @@
       <c r="A13" s="63">
         <v>10</v>
       </c>
-      <c r="B13" s="84"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="59"/>
       <c r="D13" s="71"/>
       <c r="E13" s="59"/>
@@ -2830,7 +2833,7 @@
       <c r="A14" s="63">
         <v>11</v>
       </c>
-      <c r="B14" s="86">
+      <c r="B14" s="77">
         <v>7</v>
       </c>
       <c r="C14" s="60"/>
@@ -2853,7 +2856,7 @@
       <c r="A15" s="63">
         <v>12</v>
       </c>
-      <c r="B15" s="84"/>
+      <c r="B15" s="79"/>
       <c r="C15" s="59"/>
       <c r="D15" s="71"/>
       <c r="E15" s="59"/>
@@ -2874,7 +2877,7 @@
       <c r="A16" s="63">
         <v>13</v>
       </c>
-      <c r="B16" s="86">
+      <c r="B16" s="77">
         <v>8</v>
       </c>
       <c r="C16" s="60"/>
@@ -2897,7 +2900,7 @@
       <c r="A17" s="63">
         <v>14</v>
       </c>
-      <c r="B17" s="84"/>
+      <c r="B17" s="79"/>
       <c r="C17" s="59"/>
       <c r="D17" s="71"/>
       <c r="E17" s="59"/>
@@ -2918,7 +2921,7 @@
       <c r="A18" s="63">
         <v>15</v>
       </c>
-      <c r="B18" s="86">
+      <c r="B18" s="77">
         <v>9</v>
       </c>
       <c r="C18" s="60"/>
@@ -2941,7 +2944,7 @@
       <c r="A19" s="63">
         <v>16</v>
       </c>
-      <c r="B19" s="84"/>
+      <c r="B19" s="79"/>
       <c r="C19" s="59"/>
       <c r="D19" s="71"/>
       <c r="E19" s="59"/>
@@ -3008,7 +3011,7 @@
       <c r="A22" s="63">
         <v>19</v>
       </c>
-      <c r="B22" s="82">
+      <c r="B22" s="80">
         <v>12</v>
       </c>
       <c r="C22" s="57"/>
@@ -3031,7 +3034,7 @@
       <c r="A23" s="63">
         <v>20</v>
       </c>
-      <c r="B23" s="84"/>
+      <c r="B23" s="79"/>
       <c r="C23" s="59"/>
       <c r="D23" s="71"/>
       <c r="E23" s="59"/>
@@ -3052,7 +3055,7 @@
       <c r="A24" s="63">
         <v>21</v>
       </c>
-      <c r="B24" s="86">
+      <c r="B24" s="77">
         <v>13</v>
       </c>
       <c r="C24" s="60"/>
@@ -3075,7 +3078,7 @@
       <c r="A25" s="63">
         <v>22</v>
       </c>
-      <c r="B25" s="83"/>
+      <c r="B25" s="78"/>
       <c r="C25" s="58"/>
       <c r="D25" s="73"/>
       <c r="E25" s="58"/>
@@ -3096,7 +3099,7 @@
       <c r="A26" s="63">
         <v>23</v>
       </c>
-      <c r="B26" s="84"/>
+      <c r="B26" s="79"/>
       <c r="C26" s="59"/>
       <c r="D26" s="71"/>
       <c r="E26" s="59"/>
@@ -3117,7 +3120,7 @@
       <c r="A27" s="63">
         <v>24</v>
       </c>
-      <c r="B27" s="86">
+      <c r="B27" s="77">
         <v>14</v>
       </c>
       <c r="C27" s="60"/>
@@ -3140,7 +3143,7 @@
       <c r="A28" s="63">
         <v>25</v>
       </c>
-      <c r="B28" s="83"/>
+      <c r="B28" s="78"/>
       <c r="C28" s="58"/>
       <c r="D28" s="73"/>
       <c r="E28" s="58"/>
@@ -3161,7 +3164,7 @@
       <c r="A29" s="63">
         <v>26</v>
       </c>
-      <c r="B29" s="84"/>
+      <c r="B29" s="79"/>
       <c r="C29" s="59"/>
       <c r="D29" s="71"/>
       <c r="E29" s="59"/>
@@ -3258,16 +3261,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B26"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B1:Q1"/>
     <mergeCell ref="B8:B10"/>
@@ -3282,6 +3275,16 @@
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <conditionalFormatting sqref="K1:K2 K4:K1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="5"/>
@@ -3291,7 +3294,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'اطلاعات پایه'!$G$1:$G$2</xm:f>
@@ -3310,35 +3313,29 @@
           </x14:formula1>
           <xm:sqref>J5:J8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
-          <x14:formula1>
-            <xm:f>'اطلاعات پایه'!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>H4:H5 K7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{12DC327F-9EBE-4137-A2F7-F744D102670A}">
-          <x14:formula1>
-            <xm:f>'اطلاعات پایه'!$D:$D</xm:f>
-          </x14:formula1>
-          <xm:sqref>D8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4ED068DC-E4D0-4CBB-81EA-2A865244CAED}">
-          <x14:formula1>
-            <xm:f>'اطلاعات پایه'!$C$2:$C$32</xm:f>
-          </x14:formula1>
-          <xm:sqref>C4:C29</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BAFE9CF6-FB53-4675-B22E-5C9CB7B86B2F}">
           <x14:formula1>
             <xm:f>'اطلاعات پایه'!$D$2:$D$363</xm:f>
           </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
+          <xm:sqref>D4:D8</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{11461B2A-CCA4-40A1-A2B6-850A9733E994}">
           <x14:formula1>
             <xm:f>'اطلاعات پایه'!$A$2:$A$10</xm:f>
           </x14:formula1>
           <xm:sqref>G4:G29</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+          <x14:formula1>
+            <xm:f>'اطلاعات پایه'!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>K7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4ED068DC-E4D0-4CBB-81EA-2A865244CAED}">
+          <x14:formula1>
+            <xm:f>'اطلاعات پایه'!$C$2:$C$31</xm:f>
+          </x14:formula1>
+          <xm:sqref>C4:C29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3352,7 +3349,7 @@
   <dimension ref="A1:J716"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3441,7 +3438,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
         <v>159</v>
@@ -3456,7 +3453,7 @@
         <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>160</v>
@@ -3470,7 +3467,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>70</v>
@@ -3482,7 +3479,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
         <v>161</v>
@@ -3493,7 +3490,7 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="D10" t="s">
         <v>162</v>
@@ -3502,7 +3499,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>163</v>
@@ -3510,7 +3507,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>134</v>
@@ -3519,7 +3516,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
         <v>164</v>
@@ -3527,7 +3524,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
@@ -3536,7 +3533,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
         <v>165</v>
@@ -3544,7 +3541,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
         <v>166</v>
@@ -3553,7 +3550,7 @@
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
         <v>167</v>
@@ -3561,7 +3558,7 @@
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
         <v>148</v>
@@ -3570,7 +3567,7 @@
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
         <v>168</v>
@@ -3578,7 +3575,7 @@
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
         <v>169</v>
@@ -3587,7 +3584,7 @@
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
         <v>170</v>
@@ -3595,7 +3592,7 @@
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
         <v>171</v>
@@ -3604,7 +3601,7 @@
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
         <v>172</v>
@@ -3612,7 +3609,7 @@
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
         <v>173</v>
@@ -3621,7 +3618,7 @@
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D25" t="s">
         <v>174</v>
@@ -3629,7 +3626,7 @@
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D26" t="s">
         <v>108</v>
@@ -3638,7 +3635,7 @@
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
         <v>114</v>
@@ -3646,7 +3643,7 @@
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D28" t="s">
         <v>175</v>
@@ -3655,7 +3652,7 @@
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
         <v>176</v>
@@ -3663,7 +3660,7 @@
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D30" t="s">
         <v>143</v>
@@ -3672,16 +3669,13 @@
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="32" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>61</v>
-      </c>
       <c r="D32" t="s">
         <v>178</v>
       </c>

</xml_diff>